<commit_message>
selected tools comparison (state of the art)
</commit_message>
<xml_diff>
--- a/research_study/ddos.xlsx
+++ b/research_study/ddos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vemanuele/Desktop/regressione/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vemanuele/Documents/GitHub/masters-degree-thesis/research_study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C09F387-A0F1-1A41-BB1C-26EF39F5DBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D925F7F-FC5F-CD48-947D-C7EB4BB3664F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1000" windowWidth="27640" windowHeight="15620" xr2:uid="{D6A7C2E7-8E77-2149-9251-F40823F04256}"/>
   </bookViews>
@@ -8447,7 +8447,7 @@
         <c:crossAx val="86179279"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.5"/>
+        <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="86179279"/>
@@ -9718,13 +9718,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>6625</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>13252</xdr:rowOff>
+      <xdr:rowOff>13253</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>54</xdr:col>
-      <xdr:colOff>582706</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>149411</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10051,8 +10051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{396347C2-3DA1-A645-A05F-E7881456BE4B}">
   <dimension ref="A1:D657"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="92" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19858,7 +19858,7 @@
         <v>1.9353356142277223</v>
       </c>
       <c r="D613">
-        <f t="shared" ref="D613:D676" si="20">(C613-C612)/(B613-B612)</f>
+        <f t="shared" ref="D613:D657" si="20">(C613-C612)/(B613-B612)</f>
         <v>-3.01699398862959E-5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dos attack detection (state of the art)
</commit_message>
<xml_diff>
--- a/research_study/ddos.xlsx
+++ b/research_study/ddos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vemanuele/Documents/GitHub/masters-degree-thesis/research_study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D925F7F-FC5F-CD48-947D-C7EB4BB3664F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4D04E8-BC12-0A41-B160-571D2C6B380F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1000" windowWidth="27640" windowHeight="15620" xr2:uid="{D6A7C2E7-8E77-2149-9251-F40823F04256}"/>
   </bookViews>
@@ -10051,8 +10051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{396347C2-3DA1-A645-A05F-E7881456BE4B}">
   <dimension ref="A1:D657"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>